<commit_message>
icdc regression 1 to 16 and 29 to 35
</commit_message>
<xml_diff>
--- a/InputFiles/TC02_Canine_Filter_NeutStatus-No.xlsx
+++ b/InputFiles/TC02_Canine_Filter_NeutStatus-No.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A484EC5D-72A3-402F-8618-48264379139F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808F57FC-AD3A-4BCD-8AE2-904D5B1D41D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>WebExcel</t>
   </si>
@@ -57,41 +57,6 @@
     <t>FilesTab</t>
   </si>
   <si>
-    <t xml:space="preserve">
-MATCH (f:file)--&gt;(parent)
-WITH DISTINCT f, parent
-MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
- MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
-WHERE demo.neutered_indicator IN ["No"]  
-WITH DISTINCT f, parent, c, demo, diag, s
-RETURN coalesce(f.file_name, '') AS `File Name`,
-        coalesce(f.file_type, '') AS `File Type`,
-        coalesce(labels(parent)[0], '') AS `Association`,
-        coalesce(f.file_description, '') AS `Description`,
-        coalesce(f.file_format, '') AS `Format`,
-        coalesce(f.file_size, '') AS `Size`,
-        coalesce(c.case_id, '') AS `Case ID`,
-        coalesce(demo.breed,'') AS Breed , 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
-        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)
-  WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies
-  MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies
-  MATCH (d:diagnosis)
-  WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies
-  MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis)
-    WHERE demo.neutered_indicator IN ["No"]  
-  OPTIONAL MATCH (f:file)-[*]-&gt;(c)
-  OPTIONAL MATCH (samp:sample)-[*]-&gt;(c)
-  WITH DISTINCT c AS c, p, s, demo, diag, f, samp
-  RETURN count(DISTINCT(f)) as number_of_files ,
-             count(DISTINCT(samp)) as number_of_sample ,
-             count(DISTINCT(c.case_id)) as number_of_cases ,
-             count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
-  </si>
-  <si>
     <t>TC02_Canine_Filter_NeutStatus-No_Neo4jData.xlsx</t>
   </si>
   <si>
@@ -99,12 +64,12 @@
   </si>
   <si>
     <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
-WHERE demo.neutered_indicator IN ["No"]  
+WHERE demo.neutered_indicator IN ["No"]
 WITH DISTINCT samp AS samp, c, demo, diag
 RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
         coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(demo.breed,'') AS Breed , 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
+        coalesce(demo.breed,'') AS Breed,
+        coalesce(diag.disease_term,'') AS Diagnosis, 
         coalesce(samp.sample_site, '') AS `Sample Site`,
         coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
         coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
@@ -115,23 +80,103 @@
         coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
   </si>
   <si>
+    <t>StudyFilesTab</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(s:study)
+MATCH (s)&lt;--(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis)
+WHERE demo.neutered_indicator IN ["No"] 
+WITH DISTINCT f,  s, c, demo, diag
+WITH
+        f, c, demo, diag, s,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH    
+        f, c, demo, diag, s,
+        f.file_size /(1024^i) AS value, 10^precision AS factor,
+        units[i] as unit
+WITH    
+        f,  c, demo, diag, s, unit,
+        round(factor * value)/factor AS size
+RETURN DISTINCT
+  coalesce(f.file_name, '') AS `File Name`,
+  coalesce(f.file_type, '') AS `File Type`,
+  coalesce("study", '') AS `Association`,
+  coalesce(f.file_description, '') AS `Description`,
+  coalesce(f.file_format, '') AS  Format,
+  CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+  coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
+  </si>
+  <si>
+    <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (diag:diagnosis)--&gt;(c)
+OPTIONAL MATCH (f:file)-[*]-&gt;(c)
+OPTIONAL MATCH (sf:file)--&gt;(s)
+WITH DISTINCT f, sf, samp AS samp, c, demo, diag, s, p
+WHERE demo.neutered_indicator IN ["No"]
+RETURN  
+    count(distinct p) AS Programs,
+    count(distinct s) AS Studies,
+    count(distinct c) AS Cases,
+    count(distinct samp) AS Samples,
+    count(distinct f) AS `Case Files`,
+    count(distinct sf) AS `Study Files`</t>
+  </si>
+  <si>
     <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+WHERE demo.neutered_indicator IN ["No"]
 MATCH (c)&lt;--(diag:diagnosis)
 OPTIONAL MATCH (samp:sample)--&gt;(c)
 OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
-WITH DISTINCT c, s, demo, diag, co
-WHERE demo.neutered_indicator IN ["No"]  
-RETURN  coalesce(c.case_id, '') AS `Case ID` ,
-        coalesce(s.clinical_study_designation, '') AS `Study Code` ,
-        coalesce(s.clinical_study_type, '') AS  `Study Type`,
-        coalesce(demo.breed, '') AS Breed ,
-        coalesce(diag.disease_term, '') AS Diagnosis ,
-        coalesce(diag.stage_of_disease, '') AS `Stage of Disease` ,
-        coalesce(demo.patient_age_at_enrollment, '') AS Age ,
-        coalesce(demo.sex, '') AS Sex ,
-        coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
-        coalesce(demo.weight, '') AS `Weight (kg)`,
-        coalesce(diag.best_response, '') AS `Response to Treatment`</t>
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age
+RETURN  
+       coalesce(c.case_id, '') AS `Case ID`,
+       coalesce(s.clinical_study_designation, '') AS `Study Code`,
+       coalesce(s.clinical_study_type, '') AS  `Study Type`,
+       coalesce(demo.breed, '') AS Breed ,
+       coalesce(diag.disease_term, '') AS Diagnosis ,
+       coalesce(diag.stage_of_disease, '') AS `Stage of Disease`,
+       CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END AS Age,
+       coalesce(demo.sex, '') AS Sex,
+       coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
+ coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `Weight (kg)`,
+       coalesce(diag.best_response, '') AS `Response to Treatment`,
+       coalesce(co.cohort_description, '') AS `Cohort`</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(parent)
+WITH DISTINCT f, parent
+MATCH (diag:diagnosis)--&gt;(c)
+OPTIONAL MATCH (f)-[*]-&gt;(samp:sample)
+MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
+WHERE demo.neutered_indicator IN ["No"] 
+OPTIONAL MATCH (s:study)&lt;--(c)&lt;--(diag:diagnosis)&lt;-[*]-(samp:sample)
+WITH
+        f, parent, c, demo, diag, s, samp,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH
+        f, parent, c, demo, diag, s, samp,
+        f.file_size /(1024^i) AS value, 
+        10^precision AS factor,
+        units[i] as unit
+WITH    
+        f, parent, c, demo, diag, s, samp, unit,
+        round(factor * value)/factor AS size
+RETURN 
+        coalesce(f.file_name, '') AS `File Name`,
+        coalesce(f.file_type, '') AS `File Type`,
+        coalesce(labels(parent)[0], '') AS `Association`,
+        coalesce(f.file_description, '') AS `Description`,
+        coalesce(f.file_format, '') AS `Format`,
+        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+        coalesce(samp.sample_id, '') AS `Sample ID`,
+        coalesce(c.case_id, '') AS `Case ID`,
+        coalesce(demo.breed,'') AS Breed ,
+        coalesce(diag.disease_term,'') AS Diagnosis</t>
   </si>
 </sst>
 </file>
@@ -501,22 +546,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="87.6640625" customWidth="1"/>
-    <col min="3" max="3" width="75.77734375" customWidth="1"/>
-    <col min="4" max="4" width="70.21875" customWidth="1"/>
-    <col min="5" max="5" width="28.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="87.5703125" customWidth="1"/>
+    <col min="3" max="3" width="75.85546875" customWidth="1"/>
+    <col min="4" max="4" width="70.140625" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -533,55 +578,72 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="300" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="225" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="4" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="5" spans="1:5" ht="375" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>